<commit_message>
updated tracker and add solution
</commit_message>
<xml_diff>
--- a/LeetCode Tracker.xlsx
+++ b/LeetCode Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D237F2A7-6701-4B97-A61B-733161B98707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AC8A6B-C38F-456B-8389-9A4094636616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2FA590F6-CEBE-453D-A814-55EB366ADEEE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -126,6 +126,33 @@
   </si>
   <si>
     <t>LinkedList</t>
+  </si>
+  <si>
+    <t>Single Number</t>
+  </si>
+  <si>
+    <t>Bit Manupilation</t>
+  </si>
+  <si>
+    <t>Phase 4</t>
+  </si>
+  <si>
+    <t>Go back to Step 2</t>
+  </si>
+  <si>
+    <t>Phase 5</t>
+  </si>
+  <si>
+    <t>Completion of all phases</t>
+  </si>
+  <si>
+    <t>Phase 6</t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>Phase 3-4</t>
   </si>
 </sst>
 </file>
@@ -581,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECAF50C-0FA8-4FE8-AF1F-0197AD9DA707}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,6 +745,12 @@
       <c r="H6" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="K6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -744,6 +777,12 @@
       <c r="H7" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="K7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -770,6 +809,12 @@
       <c r="H8" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="K8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -820,7 +865,33 @@
         <v>8</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>19</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>136</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated tracker and new problem
</commit_message>
<xml_diff>
--- a/LeetCode Tracker.xlsx
+++ b/LeetCode Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AC733B-3C36-43C2-B97C-E004E786D59A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871DDB86-8A0B-4FE9-8EDE-D25C8DE2DA4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2FA590F6-CEBE-453D-A814-55EB366ADEEE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>Reverse Linked List</t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Linked List</t>
   </si>
 </sst>
 </file>
@@ -611,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECAF50C-0FA8-4FE8-AF1F-0197AD9DA707}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,6 +923,32 @@
         <v>8</v>
       </c>
       <c r="H12" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated tracker and notes
</commit_message>
<xml_diff>
--- a/LeetCode Tracker.xlsx
+++ b/LeetCode Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871DDB86-8A0B-4FE9-8EDE-D25C8DE2DA4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79DA882-D53F-4479-9145-BB93C834D9E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2FA590F6-CEBE-453D-A814-55EB366ADEEE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -131,9 +131,6 @@
     <t>Single Number</t>
   </si>
   <si>
-    <t>Bit Manupilation</t>
-  </si>
-  <si>
     <t>Phase 4</t>
   </si>
   <si>
@@ -159,6 +156,45 @@
   </si>
   <si>
     <t>Merge Two Sorted Linked List</t>
+  </si>
+  <si>
+    <t>Number of Good Pairs</t>
+  </si>
+  <si>
+    <t>Math/Arrays/HashMap</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>***This is not easy, new method to count elements in array.</t>
+  </si>
+  <si>
+    <t>Bit Manipulation</t>
+  </si>
+  <si>
+    <t>This is new chapter. Haven't learn yet. Brute force solution is better than all 3 previous solution except Bit Manipulation method.</t>
+  </si>
+  <si>
+    <t>This is complicated. Need to understand why for loop loops through (2*k). Example: for(int i=0; i&lt;arr.length; i+=2*k);</t>
+  </si>
+  <si>
+    <t>This is to looping by counting space, then after counted the first space, then start reversing the first word, then continue to next space. Still need to try optimal solution if possible.</t>
+  </si>
+  <si>
+    <t>This is basic, just reverse all the string with two pointers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is straightforward. I just take out the vowels into another array. Then re-insert by decrement for loop to the actual string. Should have another optimal solution. </t>
+  </si>
+  <si>
+    <t>Short code as well but need to understand foundation concept.</t>
+  </si>
+  <si>
+    <t>Even though code is short, need to understand solution.</t>
+  </si>
+  <si>
+    <t>Could use the MergeSort but be clear minded on LinkList.</t>
   </si>
 </sst>
 </file>
@@ -198,7 +234,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -210,21 +246,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -250,11 +271,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -265,18 +306,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,350 +690,442 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECAF50C-0FA8-4FE8-AF1F-0197AD9DA707}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.85546875" style="7" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="K1" s="8" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="13"/>
+      <c r="L1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="8"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="K3" s="1" t="s">
+      <c r="M1" s="11"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="L2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="K4" s="1" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
+      <c r="L3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15"/>
+      <c r="L4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="16"/>
+      <c r="L5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="16"/>
+      <c r="L6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="18"/>
+      <c r="L7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" t="s">
+    </row>
+    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>344</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>541</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>345</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>557</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>237</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>136</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>206</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>344</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F16" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G16" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>541</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="H16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>1512</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="D17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>345</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="H17" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>557</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>237</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>136</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>206</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>21</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>39</v>
+      <c r="I17" s="19" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:H4"/>
-    <mergeCell ref="K1:L2"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="A1:I7"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C1:C4 C8:C1048576">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated and added new problems
</commit_message>
<xml_diff>
--- a/LeetCode Tracker.xlsx
+++ b/LeetCode Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BFFFA8-B8AF-4EE4-A4E3-744B444F9BD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B387119-B40C-4D19-81F3-B57C949650D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2FA590F6-CEBE-453D-A814-55EB366ADEEE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -208,6 +208,15 @@
   <si>
     <t>***This is really important. Even though acceptance rate is low, need to remember how to do it and understand problem properly. This problem is between pointers and need to be clear position of pointers. This is array m+n. 
 Hint: Try to insert elements in decrement order.</t>
+  </si>
+  <si>
+    <t>Two Sums</t>
+  </si>
+  <si>
+    <t>Arrays/HashMap</t>
+  </si>
+  <si>
+    <t>***This is an important interview question as well. Because it is between x=target -y; inserting the elements into HashMap and compare from there. It seems that second part is two pointers but need to figure out how to do binary search first, since second part will always be sorted.</t>
   </si>
 </sst>
 </file>
@@ -328,6 +337,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -354,12 +369,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,16 +706,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECAF50C-0FA8-4FE8-AF1F-0197AD9DA707}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -719,32 +728,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="10"/>
-      <c r="L1" s="7" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="12"/>
+      <c r="L1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="8"/>
+      <c r="M1" s="10"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="14"/>
       <c r="L2" s="1" t="s">
         <v>17</v>
       </c>
@@ -753,15 +762,15 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="12"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14"/>
       <c r="L3" s="1" t="s">
         <v>18</v>
       </c>
@@ -770,15 +779,15 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="14"/>
       <c r="L4" s="4" t="s">
         <v>19</v>
       </c>
@@ -787,15 +796,15 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="13"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="15"/>
       <c r="L5" s="1" t="s">
         <v>32</v>
       </c>
@@ -804,15 +813,15 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="13"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="15"/>
       <c r="L6" s="1" t="s">
         <v>34</v>
       </c>
@@ -821,15 +830,15 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="15"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="17"/>
       <c r="L7" s="1" t="s">
         <v>36</v>
       </c>
@@ -867,16 +876,16 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
+      <c r="A9" s="7">
         <v>344</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -896,16 +905,16 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+      <c r="A10" s="7">
         <v>541</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -925,16 +934,16 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="A11" s="7">
         <v>345</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -954,16 +963,16 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+      <c r="A12" s="7">
         <v>557</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -983,16 +992,16 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
+      <c r="A13" s="7">
         <v>237</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -1012,16 +1021,16 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
+      <c r="A14" s="7">
         <v>136</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -1041,16 +1050,16 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
+      <c r="A15" s="7">
         <v>206</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1070,16 +1079,16 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
+      <c r="A16" s="7">
         <v>21</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -1099,16 +1108,16 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
+      <c r="A17" s="7">
         <v>1512</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="7" t="s">
         <v>42</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -1128,10 +1137,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
+      <c r="A18" s="7">
         <v>88</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -1154,6 +1163,35 @@
       </c>
       <c r="I18" s="6" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>1</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated tracker and added new solution
</commit_message>
<xml_diff>
--- a/LeetCode Tracker.xlsx
+++ b/LeetCode Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B387119-B40C-4D19-81F3-B57C949650D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A9BEC3-C8E7-4291-99D3-87C9CCB9078C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2FA590F6-CEBE-453D-A814-55EB366ADEEE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="76">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -217,6 +217,51 @@
   </si>
   <si>
     <t>***This is an important interview question as well. Because it is between x=target -y; inserting the elements into HashMap and compare from there. It seems that second part is two pointers but need to figure out how to do binary search first, since second part will always be sorted.</t>
+  </si>
+  <si>
+    <t>Valid Palindrome</t>
+  </si>
+  <si>
+    <t>O(n)?</t>
+  </si>
+  <si>
+    <t>***This is very very important!! Even though most of the people did Brute force, it is still better to find optimal solution. The Optimal Solution is testing to see if you really understand programming language in classes or not. Should really understand how the optimal solution works.</t>
+  </si>
+  <si>
+    <t>Linked List Cycle</t>
+  </si>
+  <si>
+    <t>***This is technically using two pointers to detect where each will be. This is hard because cannot think of cycle where two pointers will meet. Most probably would need to rethink or train self to count/understand how the cycle would work.</t>
+  </si>
+  <si>
+    <t>Tried</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t># Visited</t>
+  </si>
+  <si>
+    <t>Time Taken (min)</t>
+  </si>
+  <si>
+    <t>Solved</t>
+  </si>
+  <si>
+    <t>Intersection of Two LinkedList</t>
+  </si>
+  <si>
+    <t>RunTime</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
+  <si>
+    <t>***This is a very good question. At least, the solution has been understood, however, do not underestimate and keep practicing and try it again, try to understand it better so it becomes a habit to solve it.</t>
   </si>
 </sst>
 </file>
@@ -241,7 +286,7 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -317,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -343,12 +388,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -361,6 +406,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -369,6 +417,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,10 +757,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECAF50C-0FA8-4FE8-AF1F-0197AD9DA707}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="15" ySplit="8" topLeftCell="P21" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P1" sqref="P1"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,16 +772,21 @@
     <col min="2" max="2" width="27.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="59.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -738,13 +797,18 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
-      <c r="I1" s="12"/>
-      <c r="L1" s="9" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="12"/>
+      <c r="O1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="10"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P1" s="19"/>
+      <c r="Q1" s="10"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -753,15 +817,19 @@
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
-      <c r="I2" s="14"/>
-      <c r="L2" s="1" t="s">
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="14"/>
+      <c r="O2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -770,15 +838,19 @@
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
-      <c r="I3" s="14"/>
-      <c r="L3" s="1" t="s">
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="14"/>
+      <c r="O3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -787,66 +859,82 @@
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
-      <c r="I4" s="14"/>
-      <c r="L4" s="4" t="s">
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14"/>
+      <c r="O4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M4" t="s">
+      <c r="P4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
       <c r="I5" s="15"/>
-      <c r="L5" s="1" t="s">
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="16"/>
+      <c r="O5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M5" t="s">
+      <c r="P5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
       <c r="I6" s="15"/>
-      <c r="L6" s="1" t="s">
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="16"/>
+      <c r="O6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M6" t="s">
+      <c r="P6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
       <c r="I7" s="17"/>
-      <c r="L7" s="1" t="s">
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="18"/>
+      <c r="O7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M7" t="s">
+      <c r="P7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -871,11 +959,23 @@
       <c r="H8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>344</v>
       </c>
@@ -900,11 +1000,23 @@
       <c r="H9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="9">
+        <v>60</v>
+      </c>
+      <c r="L9" s="9">
+        <v>2</v>
+      </c>
+      <c r="M9" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>541</v>
       </c>
@@ -929,11 +1041,23 @@
       <c r="H10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="9">
+        <v>60</v>
+      </c>
+      <c r="L10" s="9">
+        <v>2</v>
+      </c>
+      <c r="M10" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>345</v>
       </c>
@@ -958,11 +1082,23 @@
       <c r="H11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="9">
+        <v>60</v>
+      </c>
+      <c r="L11" s="9">
+        <v>2</v>
+      </c>
+      <c r="M11" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>557</v>
       </c>
@@ -987,11 +1123,23 @@
       <c r="H12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="9">
+        <v>60</v>
+      </c>
+      <c r="L12" s="9">
+        <v>2</v>
+      </c>
+      <c r="M12" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>237</v>
       </c>
@@ -1016,11 +1164,23 @@
       <c r="H13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="9">
+        <v>60</v>
+      </c>
+      <c r="L13" s="9">
+        <v>2</v>
+      </c>
+      <c r="M13" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>136</v>
       </c>
@@ -1045,11 +1205,23 @@
       <c r="H14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="9">
+        <v>60</v>
+      </c>
+      <c r="L14" s="9">
+        <v>1</v>
+      </c>
+      <c r="M14" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>206</v>
       </c>
@@ -1074,11 +1246,23 @@
       <c r="H15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" s="9">
+        <v>60</v>
+      </c>
+      <c r="L15" s="9">
+        <v>2</v>
+      </c>
+      <c r="M15" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>21</v>
       </c>
@@ -1103,11 +1287,23 @@
       <c r="H16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K16" s="9">
+        <v>60</v>
+      </c>
+      <c r="L16" s="9">
+        <v>1</v>
+      </c>
+      <c r="M16" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>1512</v>
       </c>
@@ -1132,11 +1328,23 @@
       <c r="H17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K17" s="9">
+        <v>60</v>
+      </c>
+      <c r="L17" s="9">
+        <v>1</v>
+      </c>
+      <c r="M17" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>88</v>
       </c>
@@ -1161,11 +1369,23 @@
       <c r="H18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K18" s="9">
+        <v>60</v>
+      </c>
+      <c r="L18" s="9">
+        <v>1</v>
+      </c>
+      <c r="M18" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>1</v>
       </c>
@@ -1190,14 +1410,149 @@
       <c r="H19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K19" s="9">
         <v>60</v>
+      </c>
+      <c r="L19" s="9">
+        <v>1</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>125</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K20" s="9">
+        <v>60</v>
+      </c>
+      <c r="L20" s="9">
+        <v>1</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>141</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21" s="9">
+        <v>60</v>
+      </c>
+      <c r="L21" s="9">
+        <v>1</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>160</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K22" s="9">
+        <v>60</v>
+      </c>
+      <c r="L22" s="9">
+        <v>1</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="A1:I7"/>
+    <mergeCell ref="A1:M7"/>
+    <mergeCell ref="O1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C4 C8:C1048576">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">

</xml_diff>

<commit_message>
updated tracker and added problem
</commit_message>
<xml_diff>
--- a/LeetCode Tracker.xlsx
+++ b/LeetCode Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF39CAD-01AC-4C0F-9444-057B52C00892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF82A79-8AB6-40EB-AA3C-4721DAC78739}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2FA590F6-CEBE-453D-A814-55EB366ADEEE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="82">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -249,8 +249,59 @@
     <t>RunTime Error</t>
   </si>
   <si>
+    <t>Palindrome Numbers</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Time (min)</t>
+  </si>
+  <si>
+    <t>Time/Space Complexity</t>
+  </si>
+  <si>
+    <t>Understood solution</t>
+  </si>
+  <si>
+    <t>***This is very very important!! Even though most of the people did Brute force, it is still better to find optimal solution. The Optimal Solution is testing to see if you can find solution without relying on built-in libraries. Should really understand how the optimal solution works.</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>***This is not easy, new method to count elements in array. Better to go over and understand the optimal solution. Own code is too long and confusing, already forgot how it works, mathematically.</t>
+  </si>
+  <si>
     <r>
-      <t>****Need to practice again. This question teaches a lot of things. Need to revisit it again next week to understand how it works.
+      <t xml:space="preserve">This is new chapter. Haven't learn yet. Brute force solution is better than all 3 previous solution except Bit Manipulation method.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UPDATE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: XOR (^) is the solution and checking each number using bits/binary. For example, {1, 2, 1} means 1^ 2 ^ 1, will result in 2 because 1^ 1 = 0 and 0^2 will end up with 2. In binary form, 1^0 =0^1, in other words, becoming the number that is not the same. However, 0^0 = 1^1=2^2, which eventually will result in 0.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>***Need to practice again. This question teaches a lot of things. Need to revisit it again next week to understand how it works.
 1. When working on palindrome, we no need to reverse all the elements/everything, we just need to</t>
     </r>
     <r>
@@ -315,36 +366,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>. Also, including how to use an additional to class method.</t>
-    </r>
-  </si>
-  <si>
-    <t>Palindrome Numbers</t>
-  </si>
-  <si>
-    <t>Math</t>
-  </si>
-  <si>
-    <t>Time (min)</t>
-  </si>
-  <si>
-    <t>Time/Space Complexity</t>
-  </si>
-  <si>
-    <t>Understood solution</t>
-  </si>
-  <si>
-    <t>***This is very very important!! Even though most of the people did Brute force, it is still better to find optimal solution. The Optimal Solution is testing to see if you can find solution without relying on built-in libraries. Should really understand how the optimal solution works.</t>
-  </si>
-  <si>
-    <t>Master</t>
-  </si>
-  <si>
-    <t>***This is not easy, new method to count elements in array. Better to go over and understand the optimal solution. Own code is too long and confusing, already forgot how it works, mathematically.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This is new chapter. Haven't learn yet. Brute force solution is better than all 3 previous solution except Bit Manipulation method.
+      <t xml:space="preserve">. Also, including how to use an additional to class method.
 </t>
     </r>
     <r>
@@ -366,8 +388,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: XOR (^) is the solution and checking each number using bits/binary. For example, {1, 2, 1} means 1^ 2 ^ 1, will result in 2 because 1^ 1 = 0 and 0^2 will end up with 2. In binary form, 1^0 =0^1, in other words, becoming the number that is not the same. However, 0^0 = 1^1=2^2, which eventually will result in 0.</t>
+      <t>: Finally able to work on solution, but there is an optimal solution left to master! Optimal solution is using one pointer instead of two pointer. Also, optimal solution will count the length of linked list first and then divide by two to get first and second half of linked list to compare.</t>
     </r>
+  </si>
+  <si>
+    <t>***Still haven't able to understand the solution, but starting to see the picture in separating integers into digits. Bascially, taking the remainder, and multiply by 10 to get back results. 
+For example, 121. When reversed using remainder after multiple by 10, it will become 1*10 = 10 and 121/10 will become 12. This method is to remove and reduced left half of integer and append/increased right half of integer after reversing. If still confused : https://www.youtube.com/watch?v=IKY7BTa4aq8</t>
   </si>
 </sst>
 </file>
@@ -534,7 +560,119 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -889,10 +1027,10 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="17" ySplit="8" topLeftCell="R12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="17" ySplit="8" topLeftCell="R23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="P1" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
+      <selection pane="bottomRight" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +1099,7 @@
         <v>17</v>
       </c>
       <c r="R2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1007,7 +1145,7 @@
         <v>19</v>
       </c>
       <c r="R4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1111,7 +1249,7 @@
         <v>65</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>64</v>
@@ -1120,7 +1258,7 @@
         <v>35</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>1</v>
@@ -1157,9 +1295,6 @@
       <c r="J9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K9" s="9">
-        <v>60</v>
-      </c>
       <c r="L9" s="9">
         <v>2</v>
       </c>
@@ -1204,13 +1339,13 @@
       <c r="J10" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K10" s="9">
-        <v>60</v>
-      </c>
       <c r="L10" s="9">
         <v>1</v>
       </c>
       <c r="M10" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="N10" s="11" t="s">
         <v>63</v>
       </c>
       <c r="O10" s="6" t="s">
@@ -1248,14 +1383,14 @@
       <c r="J11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K11" s="9">
-        <v>60</v>
-      </c>
       <c r="L11" s="9">
         <v>2</v>
       </c>
       <c r="M11" s="11" t="s">
         <v>62</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="O11" s="6" t="s">
         <v>46</v>
@@ -1292,14 +1427,14 @@
       <c r="J12" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="9">
-        <v>60</v>
-      </c>
       <c r="L12" s="9">
         <v>2</v>
       </c>
       <c r="M12" s="11" t="s">
         <v>62</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="O12" s="6" t="s">
         <v>44</v>
@@ -1336,9 +1471,6 @@
       <c r="J13" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K13" s="9">
-        <v>60</v>
-      </c>
       <c r="L13" s="9">
         <v>2</v>
       </c>
@@ -1383,9 +1515,6 @@
       <c r="J14" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K14" s="9">
-        <v>60</v>
-      </c>
       <c r="L14" s="9">
         <v>1</v>
       </c>
@@ -1396,7 +1525,7 @@
         <v>63</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1430,9 +1559,6 @@
       <c r="J15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="9">
-        <v>60</v>
-      </c>
       <c r="L15" s="9">
         <v>2</v>
       </c>
@@ -1477,9 +1603,6 @@
       <c r="J16" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K16" s="9">
-        <v>60</v>
-      </c>
       <c r="L16" s="9">
         <v>1</v>
       </c>
@@ -1524,17 +1647,17 @@
       <c r="J17" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K17" s="9">
-        <v>60</v>
-      </c>
       <c r="L17" s="9">
         <v>1</v>
       </c>
       <c r="M17" s="11" t="s">
         <v>63</v>
       </c>
+      <c r="N17" s="11" t="s">
+        <v>63</v>
+      </c>
       <c r="O17" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="90" x14ac:dyDescent="0.25">
@@ -1568,13 +1691,13 @@
       <c r="J18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K18" s="9">
-        <v>60</v>
-      </c>
       <c r="L18" s="9">
         <v>1</v>
       </c>
       <c r="M18" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="N18" s="11" t="s">
         <v>63</v>
       </c>
       <c r="O18" s="6" t="s">
@@ -1612,14 +1735,14 @@
       <c r="J19" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K19" s="9">
-        <v>60</v>
-      </c>
       <c r="L19" s="9">
         <v>1</v>
       </c>
       <c r="M19" s="11" t="s">
         <v>62</v>
+      </c>
+      <c r="N19" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="O19" s="6" t="s">
         <v>56</v>
@@ -1656,9 +1779,6 @@
       <c r="J20" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K20" s="9">
-        <v>60</v>
-      </c>
       <c r="L20" s="9">
         <v>1</v>
       </c>
@@ -1669,7 +1789,7 @@
         <v>63</v>
       </c>
       <c r="O20" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -1703,13 +1823,13 @@
       <c r="J21" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="K21" s="9">
-        <v>60</v>
-      </c>
       <c r="L21" s="9">
         <v>1</v>
       </c>
       <c r="M21" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="N21" s="11" t="s">
         <v>63</v>
       </c>
       <c r="O21" s="6" t="s">
@@ -1747,20 +1867,20 @@
       <c r="J22" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="K22" s="9">
-        <v>60</v>
-      </c>
       <c r="L22" s="9">
         <v>1</v>
       </c>
       <c r="M22" s="11" t="s">
         <v>63</v>
       </c>
+      <c r="N22" s="11" t="s">
+        <v>63</v>
+      </c>
       <c r="O22" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="120" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="210" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>234</v>
       </c>
@@ -1773,37 +1893,58 @@
       <c r="D23" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="E23" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F23" s="5" t="s">
         <v>7</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="H23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="J23" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="L23" s="9">
+        <v>2</v>
       </c>
       <c r="M23" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N23" s="11" t="s">
         <v>63</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>9</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="J24" s="9" t="s">
         <v>63</v>
+      </c>
+      <c r="N24" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1812,22 +1953,30 @@
     <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C4 C8:C1048576">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",J1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N1:N1048576">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",N1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated tracker and solution
</commit_message>
<xml_diff>
--- a/LeetCode Tracker.xlsx
+++ b/LeetCode Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Desktop\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF82A79-8AB6-40EB-AA3C-4721DAC78739}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9D2A3F-8C0D-4977-B64B-D12F647BE7CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2FA590F6-CEBE-453D-A814-55EB366ADEEE}"/>
+    <workbookView xWindow="9165" yWindow="345" windowWidth="19635" windowHeight="7095" xr2:uid="{2FA590F6-CEBE-453D-A814-55EB366ADEEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="84">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -155,9 +155,6 @@
     <t>Number of Good Pairs</t>
   </si>
   <si>
-    <t>Math/Arrays/HashMap</t>
-  </si>
-  <si>
     <t>Phase</t>
   </si>
   <si>
@@ -186,9 +183,6 @@
   </si>
   <si>
     <t>Merge Sorted Arrays</t>
-  </si>
-  <si>
-    <t>Arrays/Two Pointers</t>
   </si>
   <si>
     <t>O(m+n)</t>
@@ -199,9 +193,6 @@
   </si>
   <si>
     <t>Two Sums</t>
-  </si>
-  <si>
-    <t>Arrays/HashMap</t>
   </si>
   <si>
     <t>***This is an important interview question as well. Because it is between x=target -y; inserting the elements into HashMap and compare from there. It seems that second part is two pointers but need to figure out how to do binary search first, since second part will always be sorted.</t>
@@ -395,6 +386,23 @@
     <t>***Still haven't able to understand the solution, but starting to see the picture in separating integers into digits. Bascially, taking the remainder, and multiply by 10 to get back results. 
 For example, 121. When reversed using remainder after multiple by 10, it will become 1*10 = 10 and 121/10 will become 12. This method is to remove and reduced left half of integer and append/increased right half of integer after reversing. If still confused : https://www.youtube.com/watch?v=IKY7BTa4aq8</t>
   </si>
+  <si>
+    <t>Move Zeroes</t>
+  </si>
+  <si>
+    <t>Array/Two Pointers</t>
+  </si>
+  <si>
+    <t>Array/HashMap</t>
+  </si>
+  <si>
+    <t>Math/Array/HashMap</t>
+  </si>
+  <si>
+    <t>****There are two types of solutions to this: 
+1. Two pointers i=0, j = 1 counting till the end of array.
+2. Insertion method - two pointer as well but with 1 pointer looping and fill all 0 in front with non-zeroes. After that, just change all the remaining elements with 0's. i = 0, pos = 0.</t>
+  </si>
 </sst>
 </file>
 
@@ -433,7 +441,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -490,11 +498,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -529,6 +546,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -552,6 +572,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -560,7 +583,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -578,98 +601,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1024,13 +955,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECAF50C-0FA8-4FE8-AF1F-0197AD9DA707}">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="17" ySplit="8" topLeftCell="R23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="17" ySplit="8" topLeftCell="R12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="P1" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="K23" sqref="K23"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,171 +980,172 @@
     <col min="12" max="12" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.7109375" style="11" customWidth="1"/>
     <col min="14" max="14" width="7.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="59.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="67" style="6" customWidth="1"/>
+    <col min="17" max="17" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="13"/>
-      <c r="Q1" s="20" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="20"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="12"/>
       <c r="S1" s="10"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="15"/>
-      <c r="Q2" s="1" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R2" t="s">
-        <v>74</v>
+      <c r="Q2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="15"/>
-      <c r="Q3" s="1" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R3" t="s">
+      <c r="Q3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="15"/>
-      <c r="Q4" s="4" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="R4" t="s">
-        <v>75</v>
+      <c r="Q4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="17"/>
-      <c r="Q5" s="1" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R5" t="s">
+      <c r="Q5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="17"/>
-      <c r="Q6" s="1" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="R6" t="s">
+      <c r="Q6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="19"/>
-      <c r="Q7" s="1" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="R7" t="s">
+      <c r="Q7" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1240,25 +1172,25 @@
         <v>5</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>35</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>1</v>
@@ -1290,22 +1222,22 @@
         <v>21</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L9" s="9">
         <v>2</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
@@ -1334,22 +1266,22 @@
         <v>22</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L10" s="9">
         <v>1</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O10" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="45" x14ac:dyDescent="0.25">
@@ -1378,22 +1310,22 @@
         <v>23</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L11" s="9">
         <v>2</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="45" x14ac:dyDescent="0.25">
@@ -1422,22 +1354,22 @@
         <v>26</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L12" s="9">
         <v>2</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N12" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1466,25 +1398,25 @@
         <v>36</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L13" s="9">
         <v>2</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N13" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="135" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>136</v>
       </c>
@@ -1495,7 +1427,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>10</v>
@@ -1510,22 +1442,22 @@
         <v>26</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L14" s="9">
         <v>1</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N14" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1554,22 +1486,22 @@
         <v>36</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L15" s="9">
         <v>2</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N15" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1598,25 +1530,25 @@
         <v>36</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L16" s="9">
         <v>1</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N16" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="O16" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>1512</v>
       </c>
@@ -1627,7 +1559,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>10</v>
@@ -1642,22 +1574,22 @@
         <v>36</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L17" s="9">
         <v>1</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N17" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="90" x14ac:dyDescent="0.25">
@@ -1665,19 +1597,19 @@
         <v>88</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>8</v>
@@ -1686,22 +1618,22 @@
         <v>36</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L18" s="9">
         <v>1</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N18" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O18" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -1709,13 +1641,13 @@
         <v>1</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>10</v>
@@ -1730,22 +1662,22 @@
         <v>36</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L19" s="9">
         <v>1</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N19" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O19" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -1753,7 +1685,7 @@
         <v>125</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>2</v>
@@ -1768,28 +1700,28 @@
         <v>7</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>36</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L20" s="9">
         <v>1</v>
       </c>
       <c r="M20" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N20" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O20" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -1797,7 +1729,7 @@
         <v>141</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>2</v>
@@ -1818,22 +1750,22 @@
         <v>36</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L21" s="9">
         <v>1</v>
       </c>
       <c r="M21" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N21" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -1841,7 +1773,7 @@
         <v>160</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>2</v>
@@ -1850,7 +1782,7 @@
         <v>28</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>7</v>
@@ -1862,30 +1794,30 @@
         <v>36</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L22" s="9">
         <v>1</v>
       </c>
       <c r="M22" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N22" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O22" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="210" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="195" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>234</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>2</v>
@@ -1906,22 +1838,22 @@
         <v>18</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L23" s="9">
         <v>2</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N23" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="135" x14ac:dyDescent="0.25">
@@ -1929,54 +1861,104 @@
         <v>9</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N24" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O24" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>283</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="K25" s="9">
+        <v>30</v>
+      </c>
+      <c r="L25" s="9">
+        <v>1</v>
+      </c>
+      <c r="M25" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="N25" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:O7"/>
-    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="P1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C4 C8:C1048576">
-    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",N1)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",N1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>